<commit_message>
HOTFIX #5: Fix KULIGI (poi_31) - add missing IDs and adjust opening hours to 18:00-22:00 for evening scheduling
</commit_message>
<xml_diff>
--- a/data/zakopane.xlsx
+++ b/data/zakopane.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -20,13 +20,16 @@
     <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
     <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -37,7 +40,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -45,12 +48,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -426,224 +438,228 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>ID</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Name</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Description_short</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Description_long</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Why visit</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Opening hours</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>opening_hours_seasonal</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>time_min</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>time_max</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Price</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>ticket_normal</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>ticket_reduced</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>Address</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Region</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Lat</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>Lng</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>Link do godzin</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>Link do cennika</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>Space</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>Intensity</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>weather_dependency</t>
         </is>
       </c>
-      <c r="V1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>popularity_score</t>
         </is>
       </c>
-      <c r="W1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>Must see score</t>
         </is>
       </c>
-      <c r="X1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>Peak hours</t>
         </is>
       </c>
-      <c r="Y1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>recommended_time_of_day</t>
         </is>
       </c>
-      <c r="Z1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>City</t>
         </is>
       </c>
-      <c r="AA1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>Target group</t>
         </is>
       </c>
-      <c r="AB1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>Children's age</t>
         </is>
       </c>
-      <c r="AC1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>Type of attraction</t>
         </is>
       </c>
-      <c r="AD1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>Activity_style</t>
         </is>
       </c>
-      <c r="AE1" t="inlineStr">
+      <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>crowd_level</t>
         </is>
       </c>
-      <c r="AF1" t="inlineStr">
+      <c r="AF1" s="1" t="inlineStr">
         <is>
           <t>Budget type</t>
         </is>
       </c>
-      <c r="AG1" t="inlineStr">
+      <c r="AG1" s="1" t="inlineStr">
         <is>
           <t>Seasonality of attractions</t>
         </is>
       </c>
-      <c r="AH1" t="inlineStr">
+      <c r="AH1" s="1" t="inlineStr">
         <is>
           <t>Pro_tip</t>
         </is>
       </c>
-      <c r="AI1" t="inlineStr">
+      <c r="AI1" s="1" t="inlineStr">
         <is>
           <t>parking_name</t>
         </is>
       </c>
-      <c r="AJ1" t="inlineStr">
+      <c r="AJ1" s="1" t="inlineStr">
         <is>
           <t>parking_address</t>
         </is>
       </c>
-      <c r="AK1" t="inlineStr">
+      <c r="AK1" s="1" t="inlineStr">
         <is>
           <t>parking_lat</t>
         </is>
       </c>
-      <c r="AL1" t="inlineStr">
+      <c r="AL1" s="1" t="inlineStr">
         <is>
           <t>parking_lng</t>
         </is>
       </c>
-      <c r="AM1" t="inlineStr">
+      <c r="AM1" s="1" t="inlineStr">
         <is>
           <t>parking_type</t>
         </is>
       </c>
-      <c r="AN1" t="inlineStr">
+      <c r="AN1" s="1" t="inlineStr">
         <is>
           <t>parking_walk_time_min</t>
         </is>
       </c>
-      <c r="AO1" t="inlineStr">
+      <c r="AO1" s="1" t="inlineStr">
         <is>
           <t>priority_level</t>
         </is>
       </c>
-      <c r="AP1" t="inlineStr">
+      <c r="AP1" s="1" t="inlineStr">
         <is>
           <t>kids_only</t>
         </is>
       </c>
-      <c r="AQ1" t="inlineStr">
+      <c r="AQ1" s="1" t="inlineStr">
         <is>
           <t>Tags</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr"/>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>poi_1</t>
+        </is>
+      </c>
       <c r="B2" t="inlineStr">
         <is>
           <t>Muzeum Oscypka Zakopane</t>
@@ -830,7 +846,11 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr"/>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>poi_2</t>
+        </is>
+      </c>
       <c r="B3" t="inlineStr">
         <is>
           <t>Tatrzańskie Mini Zoo</t>
@@ -1023,7 +1043,11 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr"/>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>poi_3</t>
+        </is>
+      </c>
       <c r="B4" t="inlineStr">
         <is>
           <t>Myszogród</t>
@@ -1215,7 +1239,11 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr"/>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>poi_4</t>
+        </is>
+      </c>
       <c r="B5" t="inlineStr">
         <is>
           <t>Iluzja Park</t>
@@ -1408,7 +1436,11 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr"/>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>poi_5</t>
+        </is>
+      </c>
       <c r="B6" t="inlineStr">
         <is>
           <t>Papugarnia Egzotyczne Zakopane</t>
@@ -1600,7 +1632,11 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr"/>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>poi_6</t>
+        </is>
+      </c>
       <c r="B7" t="inlineStr">
         <is>
           <t>Podwodny Świat</t>
@@ -1792,7 +1828,11 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr"/>
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>poi_7</t>
+        </is>
+      </c>
       <c r="B8" t="inlineStr">
         <is>
           <t>Zjazd pontonem ze skoczni narciarskiej Wielka Krokiew</t>
@@ -1917,7 +1957,7 @@
           <t>solo, couples, friends, family_kids</t>
         </is>
       </c>
-      <c r="AB8" s="1" t="n">
+      <c r="AB8" s="2" t="n">
         <v>41913</v>
       </c>
       <c r="AC8" t="inlineStr">
@@ -1990,7 +2030,11 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr"/>
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>poi_8</t>
+        </is>
+      </c>
       <c r="B9" t="inlineStr">
         <is>
           <t>Góralski Ślizg</t>
@@ -2191,7 +2235,11 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr"/>
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>poi_9</t>
+        </is>
+      </c>
       <c r="B10" t="inlineStr">
         <is>
           <t>Tatra Family</t>
@@ -2383,7 +2431,11 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr"/>
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>poi_10</t>
+        </is>
+      </c>
       <c r="B11" t="inlineStr">
         <is>
           <t>Park Harnasia</t>
@@ -2574,7 +2626,11 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr"/>
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>poi_11</t>
+        </is>
+      </c>
       <c r="B12" t="inlineStr">
         <is>
           <t>DINO PARK</t>
@@ -2762,7 +2818,11 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr"/>
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>poi_12</t>
+        </is>
+      </c>
       <c r="B13" t="inlineStr">
         <is>
           <t>Illusion House</t>
@@ -2953,7 +3013,11 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr"/>
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>poi_13</t>
+        </is>
+      </c>
       <c r="B14" t="inlineStr">
         <is>
           <t>Dom do góry nogami</t>
@@ -3144,7 +3208,11 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr"/>
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>poi_14</t>
+        </is>
+      </c>
       <c r="B15" t="inlineStr">
         <is>
           <t>Plac zabaw na Górnej Równi Krupowej</t>
@@ -3335,7 +3403,11 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr"/>
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>poi_15</t>
+        </is>
+      </c>
       <c r="B16" t="inlineStr">
         <is>
           <t>Termy Zakopiańskie</t>
@@ -3527,7 +3599,11 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr"/>
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>poi_16</t>
+        </is>
+      </c>
       <c r="B17" t="inlineStr">
         <is>
           <t>Termy Gorący Potok</t>
@@ -3719,7 +3795,11 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr"/>
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>poi_17</t>
+        </is>
+      </c>
       <c r="B18" t="inlineStr">
         <is>
           <t>Chochołowskie Termy</t>
@@ -3911,7 +3991,11 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr"/>
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>poi_18</t>
+        </is>
+      </c>
       <c r="B19" t="inlineStr">
         <is>
           <t>Terma Bania</t>
@@ -4102,7 +4186,11 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="inlineStr"/>
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>poi_19</t>
+        </is>
+      </c>
       <c r="B20" t="inlineStr">
         <is>
           <t>Termy Bukovina</t>
@@ -4294,7 +4382,11 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="inlineStr"/>
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>poi_20</t>
+        </is>
+      </c>
       <c r="B21" t="inlineStr">
         <is>
           <t>Wielka Krokiew</t>
@@ -4485,7 +4577,11 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="inlineStr"/>
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>poi_21</t>
+        </is>
+      </c>
       <c r="B22" t="inlineStr">
         <is>
           <t>Centrum Edukacji Przyrodniczej Tatrzańskiego Parku Narodowego</t>
@@ -4682,7 +4778,11 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr"/>
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>poi_22</t>
+        </is>
+      </c>
       <c r="B23" t="inlineStr">
         <is>
           <t>Wystawa Figur Woskowych EXPO Krupówki</t>
@@ -4873,7 +4973,11 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="inlineStr"/>
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>poi_23</t>
+        </is>
+      </c>
       <c r="B24" t="inlineStr">
         <is>
           <t>Wielka Wystawa Klocków LEGO</t>
@@ -5064,7 +5168,11 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="inlineStr"/>
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>poi_24</t>
+        </is>
+      </c>
       <c r="B25" t="inlineStr">
         <is>
           <t>Muzeum Tatrzańskie</t>
@@ -5182,7 +5290,7 @@
           <t>solo, couples, friends, seniors</t>
         </is>
       </c>
-      <c r="AB25" s="1" t="n">
+      <c r="AB25" s="2" t="n">
         <v>41913</v>
       </c>
       <c r="AC25" t="inlineStr">
@@ -5254,7 +5362,11 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="inlineStr"/>
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>poi_25</t>
+        </is>
+      </c>
       <c r="B26" t="inlineStr">
         <is>
           <t>Muzeum Kornela Makuszyńskiego</t>
@@ -5372,7 +5484,7 @@
           <t>solo, couples, friends, family_kids, seniors</t>
         </is>
       </c>
-      <c r="AB26" s="1" t="n">
+      <c r="AB26" s="2" t="n">
         <v>41913</v>
       </c>
       <c r="AC26" t="inlineStr">
@@ -5444,7 +5556,11 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="inlineStr"/>
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>poi_26</t>
+        </is>
+      </c>
       <c r="B27" t="inlineStr">
         <is>
           <t>Muzeum Stylu Zakopiańskiego im. S. Witkiewicza</t>
@@ -5562,7 +5678,7 @@
           <t>solo, couples, friends, family_kids, seniors</t>
         </is>
       </c>
-      <c r="AB27" s="1" t="n">
+      <c r="AB27" s="2" t="n">
         <v>41913</v>
       </c>
       <c r="AC27" t="inlineStr">
@@ -5634,7 +5750,11 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="inlineStr"/>
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>poi_27</t>
+        </is>
+      </c>
       <c r="B28" t="inlineStr">
         <is>
           <t>Galeria sztuki w willi Oksza</t>
@@ -5752,7 +5872,7 @@
           <t>solo, couples, friends, family_kids, seniors</t>
         </is>
       </c>
-      <c r="AB28" s="1" t="n">
+      <c r="AB28" s="2" t="n">
         <v>41913</v>
       </c>
       <c r="AC28" t="inlineStr">
@@ -5824,7 +5944,11 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="inlineStr"/>
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>poi_28</t>
+        </is>
+      </c>
       <c r="B29" t="inlineStr">
         <is>
           <t>Muzeum Karola Szymanowskiego w willi "Atma"</t>
@@ -5945,7 +6069,7 @@
           <t>solo, couples, friends, family_kids, seniors</t>
         </is>
       </c>
-      <c r="AB29" s="1" t="n">
+      <c r="AB29" s="2" t="n">
         <v>41913</v>
       </c>
       <c r="AC29" t="inlineStr">
@@ -6017,7 +6141,11 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="inlineStr"/>
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>poi_29</t>
+        </is>
+      </c>
       <c r="B30" t="inlineStr">
         <is>
           <t>Tatrzański Park Edukacyjny</t>
@@ -6216,7 +6344,11 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" t="inlineStr"/>
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>poi_30</t>
+        </is>
+      </c>
       <c r="B31" t="inlineStr">
         <is>
           <t>Kaplica Najświętszego Serca Pana Jezusa w Jaszczurówce</t>
@@ -6407,7 +6539,11 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" t="inlineStr"/>
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>poi_31</t>
+        </is>
+      </c>
       <c r="B32" t="inlineStr">
         <is>
           <t>KULIGI w Zakopanem</t>
@@ -6430,13 +6566,7 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>mon:15:00-19:00
-tue:15:00-19:00,
-wed:15:00-19:00,
-thu:15:00-19:00,
-fri:15:00-19:00,
-sat:15:00-19:00,
-sun:15:00-19:00,</t>
+          <t>mon:18:00-22:00,tue:18:00-22:00,wed:18:00-22:00,thu:18:00-22:00,fri:18:00-22:00,sat:18:00-22:00,sun:18:00-22:00</t>
         </is>
       </c>
       <c r="G32" t="inlineStr"/>

</xml_diff>

<commit_message>
CLIENT REQUEST: Usuń solo z Myszogród i Dom do góry nogami (poi_2, poi_12)
</commit_message>
<xml_diff>
--- a/data/zakopane.xlsx
+++ b/data/zakopane.xlsx
@@ -16,9 +16,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -58,12 +57,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -685,7 +685,6 @@
           <t>Sat:15:30-18:00</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr"/>
       <c r="H2" t="n">
         <v>45</v>
       </c>
@@ -882,7 +881,6 @@
 sun:8:00-20:00,</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr"/>
       <c r="H3" t="n">
         <v>30</v>
       </c>
@@ -1079,7 +1077,6 @@
 sun:10:00-19:00,</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr"/>
       <c r="H4" t="n">
         <v>30</v>
       </c>
@@ -1162,7 +1159,7 @@
       </c>
       <c r="AA4" t="inlineStr">
         <is>
-          <t>solo, couples, friends, family_kids</t>
+          <t>couples, friends, family_kids</t>
         </is>
       </c>
       <c r="AB4" t="inlineStr">
@@ -1275,7 +1272,6 @@
 sun:10:00-20:00,</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr"/>
       <c r="H5" t="n">
         <v>60</v>
       </c>
@@ -1472,7 +1468,6 @@
 sun:10:00-19:00,</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr"/>
       <c r="H6" t="n">
         <v>45</v>
       </c>
@@ -1668,7 +1663,6 @@
 sun:10:00-19:00,</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr"/>
       <c r="H7" t="n">
         <v>30</v>
       </c>
@@ -1957,7 +1951,7 @@
           <t>solo, couples, friends, family_kids</t>
         </is>
       </c>
-      <c r="AB8" s="2" t="n">
+      <c r="AB8" s="3" t="n">
         <v>41913</v>
       </c>
       <c r="AC8" t="inlineStr">
@@ -2271,7 +2265,6 @@
 sun:10:00-20:00,</t>
         </is>
       </c>
-      <c r="G10" t="inlineStr"/>
       <c r="H10" t="n">
         <v>60</v>
       </c>
@@ -2467,7 +2460,6 @@
 sun:10:00-20:00,</t>
         </is>
       </c>
-      <c r="G11" t="inlineStr"/>
       <c r="H11" t="n">
         <v>20</v>
       </c>
@@ -2662,7 +2654,6 @@
 sun:10:00-19:00,</t>
         </is>
       </c>
-      <c r="G12" t="inlineStr"/>
       <c r="H12" t="n">
         <v>60</v>
       </c>
@@ -2674,8 +2665,6 @@
           <t>brak danych</t>
         </is>
       </c>
-      <c r="K12" t="inlineStr"/>
-      <c r="L12" t="inlineStr"/>
       <c r="M12" t="inlineStr">
         <is>
           <t>Józefa Piłsudskiego, 34-500 Zakopane, Poland</t>
@@ -2854,7 +2843,6 @@
 sun:10:00-18:00,</t>
         </is>
       </c>
-      <c r="G13" t="inlineStr"/>
       <c r="H13" t="n">
         <v>45</v>
       </c>
@@ -3049,7 +3037,6 @@
 sun:10:00-18:00,</t>
         </is>
       </c>
-      <c r="G14" t="inlineStr"/>
       <c r="H14" t="n">
         <v>20</v>
       </c>
@@ -3131,7 +3118,7 @@
       </c>
       <c r="AA14" t="inlineStr">
         <is>
-          <t>solo, couples, friends, family_kids</t>
+          <t>couples, friends, family_kids</t>
         </is>
       </c>
       <c r="AB14" t="inlineStr">
@@ -3244,7 +3231,6 @@
 sun:8:00-20:00,</t>
         </is>
       </c>
-      <c r="G15" t="inlineStr"/>
       <c r="H15" t="n">
         <v>20</v>
       </c>
@@ -3439,7 +3425,6 @@
 sun:9:00-22:00,</t>
         </is>
       </c>
-      <c r="G16" t="inlineStr"/>
       <c r="H16" t="n">
         <v>90</v>
       </c>
@@ -3635,7 +3620,6 @@
 sun:9:00-22:00,</t>
         </is>
       </c>
-      <c r="G17" t="inlineStr"/>
       <c r="H17" t="n">
         <v>90</v>
       </c>
@@ -3831,7 +3815,6 @@
 sun:9:00-22:00,</t>
         </is>
       </c>
-      <c r="G18" t="inlineStr"/>
       <c r="H18" t="n">
         <v>120</v>
       </c>
@@ -4027,7 +4010,6 @@
 sun:9:00-22:00,</t>
         </is>
       </c>
-      <c r="G19" t="inlineStr"/>
       <c r="H19" t="n">
         <v>120</v>
       </c>
@@ -4222,7 +4204,6 @@
 sun:9:00-22:00,</t>
         </is>
       </c>
-      <c r="G20" t="inlineStr"/>
       <c r="H20" t="n">
         <v>120</v>
       </c>
@@ -4418,7 +4399,6 @@
 sun:9:00-17:00,</t>
         </is>
       </c>
-      <c r="G21" t="inlineStr"/>
       <c r="H21" t="n">
         <v>45</v>
       </c>
@@ -4814,7 +4794,6 @@
 sun:10:00-22:00,</t>
         </is>
       </c>
-      <c r="G23" t="inlineStr"/>
       <c r="H23" t="n">
         <v>30</v>
       </c>
@@ -5009,7 +4988,6 @@
 sun:10:00-21:00,</t>
         </is>
       </c>
-      <c r="G24" t="inlineStr"/>
       <c r="H24" t="n">
         <v>30</v>
       </c>
@@ -5204,7 +5182,6 @@
 sun:10:00-18:00,</t>
         </is>
       </c>
-      <c r="G25" t="inlineStr"/>
       <c r="H25" t="n">
         <v>60</v>
       </c>
@@ -5290,7 +5267,7 @@
           <t>solo, couples, friends, seniors</t>
         </is>
       </c>
-      <c r="AB25" s="2" t="n">
+      <c r="AB25" s="3" t="n">
         <v>41913</v>
       </c>
       <c r="AC25" t="inlineStr">
@@ -5398,7 +5375,6 @@
 sun:closed,</t>
         </is>
       </c>
-      <c r="G26" t="inlineStr"/>
       <c r="H26" t="n">
         <v>30</v>
       </c>
@@ -5484,7 +5460,7 @@
           <t>solo, couples, friends, family_kids, seniors</t>
         </is>
       </c>
-      <c r="AB26" s="2" t="n">
+      <c r="AB26" s="3" t="n">
         <v>41913</v>
       </c>
       <c r="AC26" t="inlineStr">
@@ -5592,7 +5568,6 @@
 sun:9:00-17:00,</t>
         </is>
       </c>
-      <c r="G27" t="inlineStr"/>
       <c r="H27" t="n">
         <v>45</v>
       </c>
@@ -5678,7 +5653,7 @@
           <t>solo, couples, friends, family_kids, seniors</t>
         </is>
       </c>
-      <c r="AB27" s="2" t="n">
+      <c r="AB27" s="3" t="n">
         <v>41913</v>
       </c>
       <c r="AC27" t="inlineStr">
@@ -5786,7 +5761,6 @@
 sun:9:00-17:00,</t>
         </is>
       </c>
-      <c r="G28" t="inlineStr"/>
       <c r="H28" t="n">
         <v>45</v>
       </c>
@@ -5872,7 +5846,7 @@
           <t>solo, couples, friends, family_kids, seniors</t>
         </is>
       </c>
-      <c r="AB28" s="2" t="n">
+      <c r="AB28" s="3" t="n">
         <v>41913</v>
       </c>
       <c r="AC28" t="inlineStr">
@@ -6069,7 +6043,7 @@
           <t>solo, couples, friends, family_kids, seniors</t>
         </is>
       </c>
-      <c r="AB29" s="2" t="n">
+      <c r="AB29" s="3" t="n">
         <v>41913</v>
       </c>
       <c r="AC29" t="inlineStr">
@@ -6380,7 +6354,6 @@
 sun:8:00-20:00,</t>
         </is>
       </c>
-      <c r="G31" t="inlineStr"/>
       <c r="H31" t="n">
         <v>15</v>
       </c>
@@ -6569,7 +6542,6 @@
           <t>mon:18:00-22:00,tue:18:00-22:00,wed:18:00-22:00,thu:18:00-22:00,fri:18:00-22:00,sat:18:00-22:00,sun:18:00-22:00</t>
         </is>
       </c>
-      <c r="G32" t="inlineStr"/>
       <c r="H32" t="n">
         <v>60</v>
       </c>

</xml_diff>

<commit_message>
feat: Multi-season opening hours support (CLIENT UPDATE 06.02.2026)
- Parser: _parse_seasonal_list() handles pseudo-JSON list format with regex
- Validator: find_current_season() selects matching season from list by date
- Opening hours: is_poi_open_at_time() supports List[Dict] with backward compat
- Single time: 14:00 format treated as 1-hour slot (14:00-15:00)
- Model: POI.opening_hours_seasonal type Union[List[Dict], Dict]
- Data: zakopane.xlsx updated (35/36 POI with multi-season)
- Tests: Unit tests passed (Morskie Oko 3 seasons, Muzeum Oscypka 2 seasons)
- Integration test: Both winter/summer plans generate successfully

Regex: r'([a-z_]+)\s*:\s*([^\n,]+)' successfully parses all formats
Backward compatibility: Old dict format auto-converts to single-item list
</commit_message>
<xml_diff>
--- a/data/zakopane.xlsx
+++ b/data/zakopane.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1223" uniqueCount="641">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1253" uniqueCount="662">
   <si>
     <t>ID</t>
   </si>
@@ -1598,9 +1598,6 @@
 fri:10:00-17:00,
 sat:10:00-17:00,
 sun:10:00-17:00,</t>
-  </si>
-  <si>
-    <t>Closed 13:00 - 13:30</t>
   </si>
   <si>
     <t>Bilet normalny: 15.00 zł; Bilet ulgowy: 10.00 zł</t>
@@ -1800,10 +1797,6 @@
 sun:10:00-18:00,</t>
   </si>
   <si>
-    <t>"date_from": "06-01",
-"date_to": "09-30",</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 
 mon:10:00-19:00, 
 tue:10:00-19:00, 
@@ -1814,10 +1807,6 @@
 sun:10:00-19:00,</t>
   </si>
   <si>
-    <t>"date_from": "06-01", 
-"date_to": "09-30",</t>
-  </si>
-  <si>
     <t xml:space="preserve">
 mon:8:00-16:00, 
 tue:8:00-16:00, 
@@ -1828,10 +1817,6 @@
 sun:closed,</t>
   </si>
   <si>
-    <t xml:space="preserve">"date_from": "05-01", 
-"date_to": "09-30", </t>
-  </si>
-  <si>
     <t xml:space="preserve"> 
 mon:10:00-16:00 
 tue:10:00-16:00, 
@@ -1842,10 +1827,6 @@
 sun:10:00-16:00,</t>
   </si>
   <si>
-    <t>"date_from": "04-01", 
-"date_to": "10-30",</t>
-  </si>
-  <si>
     <t xml:space="preserve">mountain_culture, regional_heritage, workshop,themed_museum     </t>
   </si>
   <si>
@@ -2102,6 +2083,455 @@
   </si>
   <si>
     <t>20.10349998425671</t>
+  </si>
+  <si>
+    <t>[
+{
+date_from: 01-01,
+date_to: 02-28,
+mon: 14:00,
+tue: 14:00,
+wed: 14:00,
+thu: 14:00,
+fri: 14:00,
+sat: 14:00,
+sun: 14:00
+},
+{
+date_from: 10-01,
+date_to: 12-30,
+mon: closed,
+tue: closed,
+wed: closed,
+thu: closed,
+fri: closed,
+sat: 15:30-18:00,
+sun: closed
+}
+]</t>
+  </si>
+  <si>
+    <t>[
+{
+date_from: 01-01,
+date_to: 12-31,
+mon:8:00-20:00,
+tue:8:00-20:00,
+wed: 8:00-20:00,
+thu:8:00-20:00,
+fri:8:00-20:00,
+sat: 8:00-20:00,
+sun:8:00-20:00
+}
+]</t>
+  </si>
+  <si>
+    <t>[
+{
+date_from: 01-01,
+date_to: 12-31,
+mon:10:00-19:00,
+tue:10:00-19:00,
+wed: 10:00-19:00,
+thu:10:00-19:00,
+fri:10:00-19:00,
+sat: 10:00-19:00,
+sun:10:00-19:00
+}
+]</t>
+  </si>
+  <si>
+    <t>[
+{
+date_from: 01-01,
+date_to: 12-31,
+mon:10:00-20:00,
+tue:10:00-20:00,
+wed: 10:00-20:00,
+thu:10:00-20:00,
+fri:10:00-20:00,
+sat: 10:00-20:00,
+sun:10:00-20:00
+}
+]</t>
+  </si>
+  <si>
+    <t>[
+{
+date_from: 06-01,
+date_to: 9-30,
+mon:9:00-17:00,
+tue:9:00-17:00,
+wed:9:00-17:00,
+thu:9:00-17:00,
+fri:11:00-19:00,
+sat:11:00-19:00,
+sun:10:00-18:00
+}
+]</t>
+  </si>
+  <si>
+    <t>[
+{
+date_from: 06-01,
+date_to: 9-30,
+mon:10:00-19:00,
+tue:10:00-19:00,
+wed: 10:00-19:00,
+thu:10:00-19:00,
+fri:10:00-19:00,
+sat: 10:00-19:00,
+sun:10:00-19:00
+}
+]</t>
+  </si>
+  <si>
+    <t>[
+{
+date_from: 01-01,
+date_to: 12-31,
+mon:10:00-20:00,
+tue:10:00-20:00,
+wed:12:00-19:00,
+thu:12:00-19:00,
+fri:12:00-19:00,
+sat: 10:00-20:00,
+sun:10:00-20:00
+}
+]</t>
+  </si>
+  <si>
+    <t>[
+{
+date_from: 01-01,
+date_to: 12-31,
+mon:10:00-18:00,
+tue:10:00-18:00,
+wed: 10:00-18:00,
+thu:10:00-18:00,
+fri:10:00-18:00,
+sat: 10:00-18:00,
+sun:10:00-18:00
+}
+]</t>
+  </si>
+  <si>
+    <t>[
+{
+date_from: 01-01,
+date_to: 12-31,
+mon:8:00-20:00,
+tue:8:00-20:00,
+wed:8:00-20:00,
+thu:8:00-20:00,
+fri:8:00-20:00,
+sat:8:00-20:00,
+sun:8:00-20:00
+}
+]</t>
+  </si>
+  <si>
+    <t>[
+{
+date_from: 01-01,
+date_to: 12-31,
+mon:9:00-22:00,
+tue:9:00-22:00,
+wed:9:00-22:00,
+thu:9:00-22:00,
+fri:9:00-22:00,
+sat:9:00-22:00,
+sun:9:00-22:00
+}
+]</t>
+  </si>
+  <si>
+    <t>[
+{
+date_from: 01-01,
+date_to: 12-31,
+mon:11:00-22:00,
+tue:11:00-22:00,
+wed:11:00-22:00,
+thu:11:00-22:00,
+fri:11:00-22:00,
+sat:9:00-22:00,
+sun:9:00-22:00
+}
+]</t>
+  </si>
+  <si>
+    <t>[
+{
+date_from: 01-01,
+date_to: 12-31,
+mon:9:00-17:00,
+tue:9:00-17:00,
+wed:9:00-17:00,
+thu:9:00-17:00,
+fri:9:00-17:00,
+sat:9:00-17:00,
+sun:9:00-17:00
+}
+]</t>
+  </si>
+  <si>
+    <t>[
+{
+date_from: 05-01,
+date_to: 09-30,
+mon:8:00-16:00,
+tue:8:00-16:00,
+wed:8:00-16:00,
+thu:8:00-16:00,
+fri:8:00-16:00,
+sat:8:00-16:00,
+sun:closed,
+}
+]</t>
+  </si>
+  <si>
+    <t>[
+{
+date_from: 01-01,
+date_to: 12-31,
+mon:10:00-22:00,
+tue:10:00-22:00,
+wed:10:00-22:00,
+thu:10:00-22:00,
+fri:10:00-22:00,
+sat:10:00-22:00,
+sun:10:00-22:00
+}
+]</t>
+  </si>
+  <si>
+    <t>[
+{
+date_from: 01-01,
+date_to: 12-31,
+mon:10:00-21:00,
+tue:10:00-21:00,
+wed:10:00-21:00,
+thu:10:00-21:00,
+fri:10:00-21:00,
+sat:10:00-21:00,
+sun:10:00-21:00
+}
+]</t>
+  </si>
+  <si>
+    <t>[
+{
+date_from: 01-01,
+date_to: 12-31,
+mon:closed,
+tue:closed,
+wed:10:00-18:00,
+thu:10:00-18:00,
+fri:10:00-18:00,
+sat:10:00-18:00,
+sun:10:00-18:00
+}
+]</t>
+  </si>
+  <si>
+    <t>[
+{
+date_from: 01-01,
+date_to: 12-31,
+mon:closed,
+tue:9:00-17:00,
+wed:9:00-17:00,
+thu:9:00-17:00,
+fri:9:00-17:00,
+sat:9:00-17:00,
+sun:closed
+}
+]</t>
+  </si>
+  <si>
+    <t>[
+{
+date_from: 01-01,
+date_to: 12-31,
+mon:9:00-17:00,
+tue:closed,
+wed:9:00-17:00,
+thu:9:00-17:00,
+fri:11:00-19:00,
+sat:11:00-19:00,
+sun:9:00-17:00
+}
+]</t>
+  </si>
+  <si>
+    <t>[
+{
+date_from: 01-01,
+date_to: 12-31,
+mon:closed,
+tue:9:00-17:00,
+wed:9:00-17:00,
+thu:9:00-17:00,
+fri:11:00-19:00,
+sat:11:00-19:00,
+sun:9:00-17:00
+}
+]</t>
+  </si>
+  <si>
+    <t>[
+{
+date_from: 01-01,
+date_to: 12-31,
+mon:closed,
+tue:10:00-17:00,
+wed:10:00-17:00,
+thu:10:00-17:00,
+fri:10:00-17:00,
+sat:10:00-17:00,
+sun:10:00-17:00,
+}
+]</t>
+  </si>
+  <si>
+    <t>[
+{
+date_from: 01-17,
+date_to: 10-30,
+mon:10:00-16:00
+tue:10:00-16:00,
+wed:10:00-16:00,
+thu:10:00-16:00,
+fri:10:00-16:00,
+sat:10:00-16:00,
+sun:10:00-16:00,
+}
+]</t>
+  </si>
+  <si>
+    <t>[
+{
+date_from: 01-01,
+date_to: 12-31,
+mon:8:00-20:00
+tue:8:00-20:00,
+wed:8:00-20:00,
+thu:8:00-20:00,
+fri:8:00-20:00,
+sat:8:00-20:00,
+sun:8:00-20:00
+}
+]</t>
+  </si>
+  <si>
+    <t>[
+  {
+    date_from: 01-01,
+    date_to: 02-28,
+   mon:15:00-19:00
+tue:15:00-19:00,
+wed:15:00-19:00,
+thu:15:00-19:00,
+fri:15:00-19:00,
+sat:15:00-19:00,
+sun:15:00-19:00
+  },
+  {
+    date_from: 12-01,
+    date_to: 12-30,
+   mon:15:00-19:00
+tue:15:00-19:00,
+wed:15:00-19:00,
+thu:15:00-19:00,
+fri:15:00-19:00,
+sat:15:00-19:00,
+sun:15:00-19:00
+  }
+]</t>
+  </si>
+  <si>
+    <t>mon:7:00-20:00
+tue:7:00-20:00,
+wed:7:00-20:00,
+thu:7:00-20:00,
+fri:7:00-20:00,
+sat:7:00-20:00,
+sun:7:00-20:00,</t>
+  </si>
+  <si>
+    <t>[
+  {
+    date_from: 01-01,
+    date_to: 03-30,
+   mon:08:00-16:00
+tue:08:00-16:00,
+wed:08:00-16:00,
+thu:08:00-16:00,
+fri:08:00-16:00,
+sat:08:00-16:00,
+sun:08:00-16:00
+  },
+  {
+    date_from: 04-01,
+    date_to: 08-30,
+   mon:07:00-20:00,
+tue:07:00-20:00,
+wed:07:00-20:00,
+thu:07:00-20:00,
+fri:07:00-20:00,
+sat:07:00-20:00,
+sun:07:00-20:00,
+  },
+ {
+    date_from: 09-01,
+    date_to: 12-30,
+   mon:08:00-20:00,
+tue:08:00-17:00,
+wed:08:00-17:00,
+thu:08:00-17:00,
+fri:08:00-17:00,
+sat:08:00-17:00,
+sun:08:00-17:00,
+}]</t>
+  </si>
+  <si>
+    <t>[
+  {
+    date_from: 01-01,
+    date_to: 03-30,
+   mon:08:00-16:00
+tue:08:00-16:00,
+wed:08:00-16:00,
+thu:08:00-16:00,
+fri:08:00-16:00,
+sat:08:00-16:00,
+sun:08:00-16:00
+  },
+  {
+    date_from: 04-01,
+    date_to: 08-30,
+   mon:07:00-20:00,
+tue:07:00-20:00,
+wed:07:00-20:00,
+thu:07:00-20:00,
+fri:07:00-20:00,
+sat:07:00-20:00,
+sun:07:00-20:00
+  },
+ {
+    date_from: 09-01,
+    date_to: 12-30,
+   mon:08:00-20:00,
+tue:08:00-17:00,
+wed:08:00-17:00,
+thu:08:00-17:00,
+fri:08:00-17:00,
+sat:08:00-17:00,
+sun:08:00-17:00
+  }
+]</t>
   </si>
 </sst>
 </file>
@@ -2587,8 +3017,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AQ37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W37" workbookViewId="0">
-      <selection activeCell="Z37" sqref="Z37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J42" sqref="J37:J42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2736,7 +3166,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:43" ht="172.2" thickBot="1">
+    <row r="2" spans="1:43" ht="317.39999999999998" thickBot="1">
       <c r="B2" s="4" t="s">
         <v>42</v>
       </c>
@@ -2752,7 +3182,9 @@
       <c r="F2" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="G2" s="5"/>
+      <c r="G2" s="4" t="s">
+        <v>636</v>
+      </c>
       <c r="H2" s="4">
         <v>45</v>
       </c>
@@ -2859,7 +3291,7 @@
         <v>74</v>
       </c>
       <c r="AQ2" s="4" t="s">
-        <v>556</v>
+        <v>551</v>
       </c>
     </row>
     <row r="3" spans="1:43" ht="172.2" thickBot="1">
@@ -2878,7 +3310,9 @@
       <c r="F3" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="G3" s="5"/>
+      <c r="G3" s="4" t="s">
+        <v>637</v>
+      </c>
       <c r="H3" s="4">
         <v>30</v>
       </c>
@@ -2985,10 +3419,10 @@
         <v>74</v>
       </c>
       <c r="AQ3" s="4" t="s">
-        <v>557</v>
+        <v>552</v>
       </c>
     </row>
-    <row r="4" spans="1:43" ht="159" thickBot="1">
+    <row r="4" spans="1:43" ht="172.2" thickBot="1">
       <c r="B4" s="4" t="s">
         <v>97</v>
       </c>
@@ -3004,7 +3438,9 @@
       <c r="F4" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="G4" s="5"/>
+      <c r="G4" s="4" t="s">
+        <v>638</v>
+      </c>
       <c r="H4" s="4">
         <v>30</v>
       </c>
@@ -3063,7 +3499,7 @@
         <v>59</v>
       </c>
       <c r="AA4" s="4" t="s">
-        <v>558</v>
+        <v>553</v>
       </c>
       <c r="AB4" s="4" t="s">
         <v>61</v>
@@ -3111,7 +3547,7 @@
         <v>74</v>
       </c>
       <c r="AQ4" s="4" t="s">
-        <v>559</v>
+        <v>554</v>
       </c>
     </row>
     <row r="5" spans="1:43" ht="198.6" thickBot="1">
@@ -3130,7 +3566,9 @@
       <c r="F5" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="G5" s="5"/>
+      <c r="G5" s="4" t="s">
+        <v>639</v>
+      </c>
       <c r="H5" s="4">
         <v>60</v>
       </c>
@@ -3237,10 +3675,10 @@
         <v>74</v>
       </c>
       <c r="AQ5" s="4" t="s">
-        <v>561</v>
+        <v>556</v>
       </c>
     </row>
-    <row r="6" spans="1:43" ht="159" thickBot="1">
+    <row r="6" spans="1:43" ht="172.2" thickBot="1">
       <c r="B6" s="4" t="s">
         <v>135</v>
       </c>
@@ -3256,7 +3694,9 @@
       <c r="F6" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="G6" s="5"/>
+      <c r="G6" s="4" t="s">
+        <v>638</v>
+      </c>
       <c r="H6" s="4">
         <v>45</v>
       </c>
@@ -3363,7 +3803,7 @@
         <v>74</v>
       </c>
       <c r="AQ6" s="4" t="s">
-        <v>562</v>
+        <v>557</v>
       </c>
     </row>
     <row r="7" spans="1:43" ht="172.2" thickBot="1">
@@ -3382,7 +3822,9 @@
       <c r="F7" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="G7" s="5"/>
+      <c r="G7" s="4" t="s">
+        <v>638</v>
+      </c>
       <c r="H7" s="4">
         <v>30</v>
       </c>
@@ -3489,7 +3931,7 @@
         <v>74</v>
       </c>
       <c r="AQ7" s="4" t="s">
-        <v>563</v>
+        <v>558</v>
       </c>
     </row>
     <row r="8" spans="1:43" ht="185.4" thickBot="1">
@@ -3506,10 +3948,10 @@
         <v>168</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>548</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>549</v>
+        <v>547</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>640</v>
       </c>
       <c r="H8" s="4">
         <v>30</v>
@@ -3617,10 +4059,10 @@
         <v>74</v>
       </c>
       <c r="AQ8" s="4" t="s">
-        <v>564</v>
+        <v>559</v>
       </c>
     </row>
-    <row r="9" spans="1:43" ht="145.80000000000001" thickBot="1">
+    <row r="9" spans="1:43" ht="172.2" thickBot="1">
       <c r="B9" s="4" t="s">
         <v>185</v>
       </c>
@@ -3634,10 +4076,10 @@
         <v>188</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>550</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>551</v>
+        <v>548</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>641</v>
       </c>
       <c r="H9" s="4">
         <v>10</v>
@@ -3745,10 +4187,10 @@
         <v>74</v>
       </c>
       <c r="AQ9" s="4" t="s">
-        <v>565</v>
+        <v>560</v>
       </c>
     </row>
-    <row r="10" spans="1:43" ht="159" thickBot="1">
+    <row r="10" spans="1:43" ht="172.2" thickBot="1">
       <c r="B10" s="4" t="s">
         <v>201</v>
       </c>
@@ -3764,7 +4206,9 @@
       <c r="F10" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="G10" s="5"/>
+      <c r="G10" s="4" t="s">
+        <v>642</v>
+      </c>
       <c r="H10" s="4">
         <v>60</v>
       </c>
@@ -3871,18 +4315,18 @@
         <v>74</v>
       </c>
       <c r="AQ10" s="4" t="s">
-        <v>566</v>
+        <v>561</v>
       </c>
     </row>
-    <row r="11" spans="1:43" ht="119.4" thickBot="1">
+    <row r="11" spans="1:43" ht="172.2" thickBot="1">
       <c r="B11" s="4" t="s">
         <v>218</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>567</v>
+        <v>562</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>568</v>
+        <v>563</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>219</v>
@@ -3890,7 +4334,9 @@
       <c r="F11" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="G11" s="5"/>
+      <c r="G11" s="4" t="s">
+        <v>639</v>
+      </c>
       <c r="H11" s="4">
         <v>20</v>
       </c>
@@ -3997,7 +4443,7 @@
         <v>74</v>
       </c>
       <c r="AQ11" s="4" t="s">
-        <v>569</v>
+        <v>564</v>
       </c>
     </row>
     <row r="12" spans="1:43" ht="185.4" thickBot="1">
@@ -4016,7 +4462,9 @@
       <c r="F12" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="G12" s="5"/>
+      <c r="G12" s="4" t="s">
+        <v>638</v>
+      </c>
       <c r="H12" s="4">
         <v>60</v>
       </c>
@@ -4119,7 +4567,7 @@
         <v>74</v>
       </c>
       <c r="AQ12" s="4" t="s">
-        <v>570</v>
+        <v>565</v>
       </c>
     </row>
     <row r="13" spans="1:43" ht="185.4" thickBot="1">
@@ -4138,7 +4586,9 @@
       <c r="F13" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="G13" s="5"/>
+      <c r="G13" s="4" t="s">
+        <v>643</v>
+      </c>
       <c r="H13" s="4">
         <v>45</v>
       </c>
@@ -4245,7 +4695,7 @@
         <v>74</v>
       </c>
       <c r="AQ13" s="4" t="s">
-        <v>571</v>
+        <v>566</v>
       </c>
     </row>
     <row r="14" spans="1:43" ht="15" thickBot="1">
@@ -4308,7 +4758,9 @@
       <c r="F15" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="G15" s="5"/>
+      <c r="G15" s="4" t="s">
+        <v>643</v>
+      </c>
       <c r="H15" s="4">
         <v>20</v>
       </c>
@@ -4415,10 +4867,10 @@
         <v>74</v>
       </c>
       <c r="AQ15" s="4" t="s">
-        <v>560</v>
+        <v>555</v>
       </c>
     </row>
-    <row r="16" spans="1:43" ht="159" thickBot="1">
+    <row r="16" spans="1:43" ht="172.2" thickBot="1">
       <c r="B16" s="4" t="s">
         <v>271</v>
       </c>
@@ -4434,7 +4886,9 @@
       <c r="F16" s="4" t="s">
         <v>275</v>
       </c>
-      <c r="G16" s="5"/>
+      <c r="G16" s="4" t="s">
+        <v>644</v>
+      </c>
       <c r="H16" s="4">
         <v>20</v>
       </c>
@@ -4541,7 +4995,7 @@
         <v>285</v>
       </c>
       <c r="AQ16" s="4" t="s">
-        <v>572</v>
+        <v>567</v>
       </c>
     </row>
     <row r="17" spans="2:43" ht="185.4" thickBot="1">
@@ -4560,7 +5014,9 @@
       <c r="F17" s="4" t="s">
         <v>290</v>
       </c>
-      <c r="G17" s="5"/>
+      <c r="G17" s="4" t="s">
+        <v>645</v>
+      </c>
       <c r="H17" s="4">
         <v>90</v>
       </c>
@@ -4667,7 +5123,7 @@
         <v>74</v>
       </c>
       <c r="AQ17" s="4" t="s">
-        <v>573</v>
+        <v>568</v>
       </c>
     </row>
     <row r="18" spans="2:43" ht="198.6" thickBot="1">
@@ -4686,7 +5142,9 @@
       <c r="F18" s="4" t="s">
         <v>305</v>
       </c>
-      <c r="G18" s="5"/>
+      <c r="G18" s="4" t="s">
+        <v>646</v>
+      </c>
       <c r="H18" s="4">
         <v>90</v>
       </c>
@@ -4793,7 +5251,7 @@
         <v>74</v>
       </c>
       <c r="AQ18" s="4" t="s">
-        <v>574</v>
+        <v>569</v>
       </c>
     </row>
     <row r="19" spans="2:43" ht="198.6" thickBot="1">
@@ -4812,7 +5270,9 @@
       <c r="F19" s="4" t="s">
         <v>290</v>
       </c>
-      <c r="G19" s="5"/>
+      <c r="G19" s="4" t="s">
+        <v>645</v>
+      </c>
       <c r="H19" s="4">
         <v>120</v>
       </c>
@@ -4919,7 +5379,7 @@
         <v>74</v>
       </c>
       <c r="AQ19" s="4" t="s">
-        <v>575</v>
+        <v>570</v>
       </c>
     </row>
     <row r="20" spans="2:43" ht="198.6" thickBot="1">
@@ -4938,7 +5398,9 @@
       <c r="F20" s="4" t="s">
         <v>290</v>
       </c>
-      <c r="G20" s="5"/>
+      <c r="G20" s="4" t="s">
+        <v>645</v>
+      </c>
       <c r="H20" s="4">
         <v>120</v>
       </c>
@@ -5045,7 +5507,7 @@
         <v>74</v>
       </c>
       <c r="AQ20" s="4" t="s">
-        <v>576</v>
+        <v>571</v>
       </c>
     </row>
     <row r="21" spans="2:43" ht="185.4" thickBot="1">
@@ -5064,7 +5526,9 @@
       <c r="F21" s="4" t="s">
         <v>290</v>
       </c>
-      <c r="G21" s="5"/>
+      <c r="G21" s="4" t="s">
+        <v>645</v>
+      </c>
       <c r="H21" s="4">
         <v>120</v>
       </c>
@@ -5171,7 +5635,7 @@
         <v>74</v>
       </c>
       <c r="AQ21" s="4" t="s">
-        <v>575</v>
+        <v>570</v>
       </c>
     </row>
     <row r="22" spans="2:43" ht="238.2" thickBot="1">
@@ -5190,7 +5654,9 @@
       <c r="F22" s="4" t="s">
         <v>370</v>
       </c>
-      <c r="G22" s="5"/>
+      <c r="G22" s="4" t="s">
+        <v>647</v>
+      </c>
       <c r="H22" s="4">
         <v>45</v>
       </c>
@@ -5297,7 +5763,7 @@
         <v>74</v>
       </c>
       <c r="AQ22" s="4" t="s">
-        <v>577</v>
+        <v>572</v>
       </c>
     </row>
     <row r="23" spans="2:43" ht="172.2" thickBot="1">
@@ -5314,10 +5780,10 @@
         <v>385</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>552</v>
-      </c>
-      <c r="G23" s="5" t="s">
-        <v>553</v>
+        <v>549</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>648</v>
       </c>
       <c r="H23" s="4">
         <v>60</v>
@@ -5425,10 +5891,10 @@
         <v>74</v>
       </c>
       <c r="AQ23" s="4" t="s">
-        <v>582</v>
+        <v>577</v>
       </c>
     </row>
-    <row r="24" spans="2:43" ht="145.80000000000001" thickBot="1">
+    <row r="24" spans="2:43" ht="172.2" thickBot="1">
       <c r="B24" s="4" t="s">
         <v>396</v>
       </c>
@@ -5444,7 +5910,9 @@
       <c r="F24" s="4" t="s">
         <v>400</v>
       </c>
-      <c r="G24" s="5"/>
+      <c r="G24" s="4" t="s">
+        <v>649</v>
+      </c>
       <c r="H24" s="4">
         <v>30</v>
       </c>
@@ -5551,10 +6019,10 @@
         <v>74</v>
       </c>
       <c r="AQ24" s="4" t="s">
-        <v>583</v>
+        <v>578</v>
       </c>
     </row>
-    <row r="25" spans="2:43" ht="145.80000000000001" thickBot="1">
+    <row r="25" spans="2:43" ht="172.2" thickBot="1">
       <c r="B25" s="4" t="s">
         <v>413</v>
       </c>
@@ -5570,7 +6038,9 @@
       <c r="F25" s="4" t="s">
         <v>417</v>
       </c>
-      <c r="G25" s="5"/>
+      <c r="G25" s="4" t="s">
+        <v>650</v>
+      </c>
       <c r="H25" s="4">
         <v>30</v>
       </c>
@@ -5677,7 +6147,7 @@
         <v>74</v>
       </c>
       <c r="AQ25" s="4" t="s">
-        <v>584</v>
+        <v>579</v>
       </c>
     </row>
     <row r="26" spans="2:43" ht="198.6" thickBot="1">
@@ -5696,7 +6166,9 @@
       <c r="F26" s="4" t="s">
         <v>432</v>
       </c>
-      <c r="G26" s="5"/>
+      <c r="G26" s="4" t="s">
+        <v>651</v>
+      </c>
       <c r="H26" s="4">
         <v>60</v>
       </c>
@@ -5803,7 +6275,7 @@
         <v>74</v>
       </c>
       <c r="AQ26" s="4" t="s">
-        <v>585</v>
+        <v>580</v>
       </c>
     </row>
     <row r="27" spans="2:43" ht="211.8" thickBot="1">
@@ -5822,7 +6294,9 @@
       <c r="F27" s="4" t="s">
         <v>447</v>
       </c>
-      <c r="G27" s="5"/>
+      <c r="G27" s="4" t="s">
+        <v>652</v>
+      </c>
       <c r="H27" s="4">
         <v>30</v>
       </c>
@@ -5929,7 +6403,7 @@
         <v>74</v>
       </c>
       <c r="AQ27" s="4" t="s">
-        <v>586</v>
+        <v>581</v>
       </c>
     </row>
     <row r="28" spans="2:43" ht="185.4" thickBot="1">
@@ -5948,7 +6422,9 @@
       <c r="F28" s="4" t="s">
         <v>462</v>
       </c>
-      <c r="G28" s="5"/>
+      <c r="G28" s="4" t="s">
+        <v>653</v>
+      </c>
       <c r="H28" s="4">
         <v>45</v>
       </c>
@@ -6055,7 +6531,7 @@
         <v>74</v>
       </c>
       <c r="AQ28" s="4" t="s">
-        <v>587</v>
+        <v>582</v>
       </c>
     </row>
     <row r="29" spans="2:43" ht="198.6" thickBot="1">
@@ -6074,7 +6550,9 @@
       <c r="F29" s="4" t="s">
         <v>476</v>
       </c>
-      <c r="G29" s="5"/>
+      <c r="G29" s="4" t="s">
+        <v>654</v>
+      </c>
       <c r="H29" s="4">
         <v>45</v>
       </c>
@@ -6181,7 +6659,7 @@
         <v>74</v>
       </c>
       <c r="AQ29" s="4" t="s">
-        <v>588</v>
+        <v>583</v>
       </c>
     </row>
     <row r="30" spans="2:43" ht="198.6" thickBot="1">
@@ -6201,7 +6679,7 @@
         <v>488</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>489</v>
+        <v>655</v>
       </c>
       <c r="H30" s="4">
         <v>30</v>
@@ -6210,7 +6688,7 @@
         <v>60</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="K30" s="4">
         <v>15</v>
@@ -6219,22 +6697,22 @@
         <v>10</v>
       </c>
       <c r="M30" s="4" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="N30" s="4" t="s">
         <v>49</v>
       </c>
       <c r="O30" s="4" t="s">
+        <v>491</v>
+      </c>
+      <c r="P30" s="4" t="s">
         <v>492</v>
       </c>
-      <c r="P30" s="4" t="s">
+      <c r="Q30" s="6" t="s">
         <v>493</v>
       </c>
-      <c r="Q30" s="6" t="s">
+      <c r="R30" s="6" t="s">
         <v>494</v>
-      </c>
-      <c r="R30" s="6" t="s">
-        <v>495</v>
       </c>
       <c r="S30" s="4" t="s">
         <v>54</v>
@@ -6282,19 +6760,19 @@
         <v>66</v>
       </c>
       <c r="AH30" s="4" t="s">
+        <v>495</v>
+      </c>
+      <c r="AI30" s="4" t="s">
         <v>496</v>
       </c>
-      <c r="AI30" s="4" t="s">
+      <c r="AJ30" s="4" t="s">
         <v>497</v>
       </c>
-      <c r="AJ30" s="4" t="s">
+      <c r="AK30" s="4" t="s">
         <v>498</v>
       </c>
-      <c r="AK30" s="4" t="s">
+      <c r="AL30" s="4" t="s">
         <v>499</v>
-      </c>
-      <c r="AL30" s="4" t="s">
-        <v>500</v>
       </c>
       <c r="AM30" s="4" t="s">
         <v>72</v>
@@ -6309,27 +6787,27 @@
         <v>74</v>
       </c>
       <c r="AQ30" s="4" t="s">
-        <v>586</v>
+        <v>581</v>
       </c>
     </row>
     <row r="31" spans="2:43" ht="172.2" thickBot="1">
       <c r="B31" s="4" t="s">
+        <v>500</v>
+      </c>
+      <c r="C31" s="4" t="s">
         <v>501</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="D31" s="4" t="s">
         <v>502</v>
       </c>
-      <c r="D31" s="4" t="s">
+      <c r="E31" s="4" t="s">
         <v>503</v>
       </c>
-      <c r="E31" s="4" t="s">
-        <v>504</v>
-      </c>
       <c r="F31" s="4" t="s">
-        <v>554</v>
-      </c>
-      <c r="G31" s="5" t="s">
-        <v>555</v>
+        <v>550</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>656</v>
       </c>
       <c r="H31" s="4">
         <v>60</v>
@@ -6338,7 +6816,7 @@
         <v>180</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="K31" s="4">
         <v>30</v>
@@ -6347,22 +6825,22 @@
         <v>25</v>
       </c>
       <c r="M31" s="4" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="N31" s="4" t="s">
         <v>49</v>
       </c>
       <c r="O31" s="4" t="s">
+        <v>506</v>
+      </c>
+      <c r="P31" s="4" t="s">
         <v>507</v>
       </c>
-      <c r="P31" s="4" t="s">
+      <c r="Q31" s="6" t="s">
         <v>508</v>
       </c>
-      <c r="Q31" s="6" t="s">
+      <c r="R31" s="6" t="s">
         <v>509</v>
-      </c>
-      <c r="R31" s="6" t="s">
-        <v>510</v>
       </c>
       <c r="S31" s="4" t="s">
         <v>85</v>
@@ -6395,7 +6873,7 @@
         <v>61</v>
       </c>
       <c r="AC31" s="4" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="AD31" s="4" t="s">
         <v>90</v>
@@ -6410,7 +6888,7 @@
         <v>179</v>
       </c>
       <c r="AH31" s="4" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="AI31" s="4" t="s">
         <v>181</v>
@@ -6419,10 +6897,10 @@
         <v>182</v>
       </c>
       <c r="AK31" s="4" t="s">
+        <v>512</v>
+      </c>
+      <c r="AL31" s="4" t="s">
         <v>513</v>
-      </c>
-      <c r="AL31" s="4" t="s">
-        <v>514</v>
       </c>
       <c r="AM31" s="4" t="s">
         <v>72</v>
@@ -6437,26 +6915,28 @@
         <v>74</v>
       </c>
       <c r="AQ31" s="4" t="s">
-        <v>589</v>
+        <v>584</v>
       </c>
     </row>
     <row r="32" spans="2:43" ht="185.4" thickBot="1">
       <c r="B32" s="4" t="s">
+        <v>514</v>
+      </c>
+      <c r="C32" s="4" t="s">
         <v>515</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="D32" s="4" t="s">
         <v>516</v>
       </c>
-      <c r="D32" s="4" t="s">
+      <c r="E32" s="4" t="s">
         <v>517</v>
       </c>
-      <c r="E32" s="4" t="s">
+      <c r="F32" s="4" t="s">
         <v>518</v>
       </c>
-      <c r="F32" s="4" t="s">
-        <v>519</v>
-      </c>
-      <c r="G32" s="5"/>
+      <c r="G32" s="4" t="s">
+        <v>657</v>
+      </c>
       <c r="H32" s="4">
         <v>15</v>
       </c>
@@ -6473,16 +6953,16 @@
         <v>0</v>
       </c>
       <c r="M32" s="4" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="N32" s="4" t="s">
         <v>49</v>
       </c>
       <c r="O32" s="4" t="s">
+        <v>520</v>
+      </c>
+      <c r="P32" s="4" t="s">
         <v>521</v>
-      </c>
-      <c r="P32" s="4" t="s">
-        <v>522</v>
       </c>
       <c r="Q32" s="4" t="s">
         <v>210</v>
@@ -6506,7 +6986,7 @@
         <v>8</v>
       </c>
       <c r="X32" s="4" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="Y32" s="4" t="s">
         <v>108</v>
@@ -6536,19 +7016,19 @@
         <v>66</v>
       </c>
       <c r="AH32" s="4" t="s">
+        <v>523</v>
+      </c>
+      <c r="AI32" s="4" t="s">
         <v>524</v>
       </c>
-      <c r="AI32" s="4" t="s">
+      <c r="AJ32" s="4" t="s">
         <v>525</v>
       </c>
-      <c r="AJ32" s="4" t="s">
+      <c r="AK32" s="4" t="s">
         <v>526</v>
       </c>
-      <c r="AK32" s="4" t="s">
+      <c r="AL32" s="4" t="s">
         <v>527</v>
-      </c>
-      <c r="AL32" s="4" t="s">
-        <v>528</v>
       </c>
       <c r="AM32" s="4" t="s">
         <v>96</v>
@@ -6563,26 +7043,28 @@
         <v>74</v>
       </c>
       <c r="AQ32" s="4" t="s">
-        <v>590</v>
+        <v>585</v>
       </c>
     </row>
-    <row r="33" spans="2:43" ht="145.80000000000001" thickBot="1">
+    <row r="33" spans="2:43" ht="317.39999999999998" thickBot="1">
       <c r="B33" s="4" t="s">
+        <v>528</v>
+      </c>
+      <c r="C33" s="4" t="s">
         <v>529</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="D33" s="4" t="s">
         <v>530</v>
       </c>
-      <c r="D33" s="4" t="s">
+      <c r="E33" s="4" t="s">
         <v>531</v>
       </c>
-      <c r="E33" s="4" t="s">
+      <c r="F33" s="4" t="s">
         <v>532</v>
       </c>
-      <c r="F33" s="4" t="s">
-        <v>533</v>
-      </c>
-      <c r="G33" s="5"/>
+      <c r="G33" s="5" t="s">
+        <v>658</v>
+      </c>
       <c r="H33" s="4">
         <v>60</v>
       </c>
@@ -6590,7 +7072,7 @@
         <v>180</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="K33" s="4">
         <v>247</v>
@@ -6599,22 +7081,22 @@
         <v>247</v>
       </c>
       <c r="M33" s="4" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="N33" s="4" t="s">
         <v>49</v>
       </c>
       <c r="O33" s="4" t="s">
+        <v>535</v>
+      </c>
+      <c r="P33" s="4" t="s">
         <v>536</v>
       </c>
-      <c r="P33" s="4" t="s">
+      <c r="Q33" s="6" t="s">
         <v>537</v>
       </c>
-      <c r="Q33" s="6" t="s">
-        <v>538</v>
-      </c>
       <c r="R33" s="6" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="S33" s="4" t="s">
         <v>85</v>
@@ -6632,7 +7114,7 @@
         <v>8</v>
       </c>
       <c r="X33" s="4" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="Y33" s="4" t="s">
         <v>58</v>
@@ -6647,7 +7129,7 @@
         <v>61</v>
       </c>
       <c r="AC33" s="4" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="AD33" s="4" t="s">
         <v>90</v>
@@ -6656,25 +7138,25 @@
         <v>64</v>
       </c>
       <c r="AF33" s="4" t="s">
+        <v>540</v>
+      </c>
+      <c r="AG33" s="4" t="s">
         <v>541</v>
       </c>
-      <c r="AG33" s="4" t="s">
+      <c r="AH33" s="4" t="s">
         <v>542</v>
       </c>
-      <c r="AH33" s="4" t="s">
+      <c r="AI33" s="12" t="s">
         <v>543</v>
       </c>
-      <c r="AI33" s="12" t="s">
+      <c r="AJ33" s="4" t="s">
         <v>544</v>
       </c>
-      <c r="AJ33" s="4" t="s">
+      <c r="AK33" s="4" t="s">
         <v>545</v>
       </c>
-      <c r="AK33" s="4" t="s">
+      <c r="AL33" s="4" t="s">
         <v>546</v>
-      </c>
-      <c r="AL33" s="4" t="s">
-        <v>547</v>
       </c>
       <c r="AM33" s="4" t="s">
         <v>72</v>
@@ -6689,24 +7171,27 @@
         <v>74</v>
       </c>
       <c r="AQ33" s="4" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="34" spans="2:43" ht="408.6" customHeight="1">
+      <c r="B34" s="13" t="s">
+        <v>573</v>
+      </c>
+      <c r="C34" s="17" t="s">
         <v>591</v>
       </c>
-    </row>
-    <row r="34" spans="2:43" ht="216">
-      <c r="B34" s="13" t="s">
-        <v>578</v>
-      </c>
-      <c r="C34" s="17" t="s">
-        <v>596</v>
-      </c>
       <c r="D34" s="14" t="s">
-        <v>600</v>
-      </c>
-      <c r="E34" s="14" t="s">
-        <v>604</v>
+        <v>595</v>
+      </c>
+      <c r="E34" s="17" t="s">
+        <v>599</v>
       </c>
       <c r="F34" s="17" t="s">
-        <v>519</v>
+        <v>659</v>
+      </c>
+      <c r="G34" s="17" t="s">
+        <v>660</v>
       </c>
       <c r="H34" s="13">
         <v>270</v>
@@ -6715,7 +7200,7 @@
         <v>350</v>
       </c>
       <c r="J34" s="13" t="s">
-        <v>623</v>
+        <v>618</v>
       </c>
       <c r="K34" s="13">
         <v>11</v>
@@ -6724,16 +7209,16 @@
         <v>5.5</v>
       </c>
       <c r="M34" s="17" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="N34" s="13" t="s">
         <v>49</v>
       </c>
       <c r="O34" s="17" t="s">
-        <v>613</v>
+        <v>608</v>
       </c>
       <c r="P34" s="17" t="s">
-        <v>617</v>
+        <v>612</v>
       </c>
       <c r="S34" s="13" t="s">
         <v>85</v>
@@ -6751,13 +7236,13 @@
         <v>9</v>
       </c>
       <c r="X34" s="13" t="s">
-        <v>624</v>
+        <v>619</v>
       </c>
       <c r="Y34" s="16" t="s">
         <v>159</v>
       </c>
       <c r="Z34" s="17" t="s">
-        <v>621</v>
+        <v>616</v>
       </c>
       <c r="AA34" s="13" t="s">
         <v>60</v>
@@ -6766,7 +7251,7 @@
         <v>61</v>
       </c>
       <c r="AC34" s="17" t="s">
-        <v>627</v>
+        <v>622</v>
       </c>
       <c r="AD34" s="13" t="s">
         <v>177</v>
@@ -6781,19 +7266,19 @@
         <v>66</v>
       </c>
       <c r="AH34" s="15" t="s">
-        <v>608</v>
+        <v>603</v>
       </c>
       <c r="AI34" s="13" t="s">
+        <v>543</v>
+      </c>
+      <c r="AJ34" s="13" t="s">
         <v>544</v>
       </c>
-      <c r="AJ34" s="13" t="s">
+      <c r="AK34" s="13" t="s">
         <v>545</v>
       </c>
-      <c r="AK34" s="13" t="s">
+      <c r="AL34" s="13" t="s">
         <v>546</v>
-      </c>
-      <c r="AL34" s="13" t="s">
-        <v>547</v>
       </c>
       <c r="AM34" s="13" t="s">
         <v>72</v>
@@ -6808,24 +7293,27 @@
         <v>74</v>
       </c>
       <c r="AQ34" s="13" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="35" spans="2:43" ht="409.6">
+      <c r="B35" s="13" t="s">
+        <v>574</v>
+      </c>
+      <c r="C35" s="17" t="s">
         <v>592</v>
       </c>
-    </row>
-    <row r="35" spans="2:43" ht="230.4">
-      <c r="B35" s="13" t="s">
-        <v>579</v>
-      </c>
-      <c r="C35" s="17" t="s">
-        <v>597</v>
-      </c>
       <c r="D35" s="14" t="s">
-        <v>601</v>
+        <v>596</v>
       </c>
       <c r="E35" s="17" t="s">
-        <v>605</v>
+        <v>600</v>
       </c>
       <c r="F35" s="17" t="s">
-        <v>519</v>
+        <v>518</v>
+      </c>
+      <c r="G35" s="14" t="s">
+        <v>661</v>
       </c>
       <c r="H35" s="13">
         <v>180</v>
@@ -6834,7 +7322,7 @@
         <v>270</v>
       </c>
       <c r="J35" s="17" t="s">
-        <v>623</v>
+        <v>618</v>
       </c>
       <c r="K35" s="13">
         <v>11</v>
@@ -6843,16 +7331,16 @@
         <v>5.5</v>
       </c>
       <c r="M35" s="17" t="s">
-        <v>625</v>
+        <v>620</v>
       </c>
       <c r="N35" s="13" t="s">
         <v>49</v>
       </c>
       <c r="O35" s="17" t="s">
-        <v>614</v>
+        <v>609</v>
       </c>
       <c r="P35" s="17" t="s">
-        <v>618</v>
+        <v>613</v>
       </c>
       <c r="S35" s="13" t="s">
         <v>85</v>
@@ -6870,13 +7358,13 @@
         <v>10</v>
       </c>
       <c r="X35" s="13" t="s">
-        <v>624</v>
+        <v>619</v>
       </c>
       <c r="Y35" s="16" t="s">
-        <v>612</v>
+        <v>607</v>
       </c>
       <c r="Z35" s="17" t="s">
-        <v>622</v>
+        <v>617</v>
       </c>
       <c r="AA35" s="17" t="s">
         <v>60</v>
@@ -6885,7 +7373,7 @@
         <v>61</v>
       </c>
       <c r="AC35" s="17" t="s">
-        <v>627</v>
+        <v>622</v>
       </c>
       <c r="AD35" s="13" t="s">
         <v>177</v>
@@ -6900,19 +7388,19 @@
         <v>66</v>
       </c>
       <c r="AH35" s="15" t="s">
-        <v>609</v>
+        <v>604</v>
       </c>
       <c r="AI35" s="13" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="AJ35" s="13" t="s">
-        <v>629</v>
+        <v>624</v>
       </c>
       <c r="AK35" s="13" t="s">
-        <v>630</v>
+        <v>625</v>
       </c>
       <c r="AL35" s="17" t="s">
-        <v>631</v>
+        <v>626</v>
       </c>
       <c r="AM35" s="13" t="s">
         <v>72</v>
@@ -6927,24 +7415,27 @@
         <v>74</v>
       </c>
       <c r="AQ35" s="13" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="36" spans="2:43" ht="409.6">
+      <c r="B36" s="13" t="s">
+        <v>575</v>
+      </c>
+      <c r="C36" s="17" t="s">
         <v>593</v>
       </c>
-    </row>
-    <row r="36" spans="2:43" ht="230.4">
-      <c r="B36" s="13" t="s">
-        <v>580</v>
-      </c>
-      <c r="C36" s="17" t="s">
-        <v>598</v>
-      </c>
       <c r="D36" s="14" t="s">
-        <v>602</v>
+        <v>597</v>
       </c>
       <c r="E36" s="17" t="s">
-        <v>606</v>
+        <v>601</v>
       </c>
       <c r="F36" s="17" t="s">
-        <v>519</v>
+        <v>518</v>
+      </c>
+      <c r="G36" s="14" t="s">
+        <v>661</v>
       </c>
       <c r="H36" s="13">
         <v>150</v>
@@ -6953,7 +7444,7 @@
         <v>240</v>
       </c>
       <c r="J36" s="17" t="s">
-        <v>623</v>
+        <v>618</v>
       </c>
       <c r="K36" s="13">
         <v>11</v>
@@ -6962,16 +7453,16 @@
         <v>5.5</v>
       </c>
       <c r="M36" s="14" t="s">
-        <v>632</v>
+        <v>627</v>
       </c>
       <c r="N36" s="13" t="s">
         <v>49</v>
       </c>
       <c r="O36" s="17" t="s">
-        <v>615</v>
+        <v>610</v>
       </c>
       <c r="P36" s="17" t="s">
-        <v>619</v>
+        <v>614</v>
       </c>
       <c r="S36" s="13" t="s">
         <v>85</v>
@@ -6989,13 +7480,13 @@
         <v>9</v>
       </c>
       <c r="X36" s="19" t="s">
-        <v>624</v>
+        <v>619</v>
       </c>
       <c r="Y36" s="16" t="s">
         <v>159</v>
       </c>
       <c r="Z36" s="17" t="s">
-        <v>580</v>
+        <v>575</v>
       </c>
       <c r="AA36" s="17" t="s">
         <v>60</v>
@@ -7004,7 +7495,7 @@
         <v>61</v>
       </c>
       <c r="AC36" s="19" t="s">
-        <v>627</v>
+        <v>622</v>
       </c>
       <c r="AD36" s="13" t="s">
         <v>177</v>
@@ -7019,19 +7510,19 @@
         <v>66</v>
       </c>
       <c r="AH36" s="15" t="s">
-        <v>610</v>
+        <v>605</v>
       </c>
       <c r="AI36" s="13" t="s">
-        <v>633</v>
+        <v>628</v>
       </c>
       <c r="AJ36" s="13" t="s">
-        <v>634</v>
+        <v>629</v>
       </c>
       <c r="AK36" s="13" t="s">
-        <v>635</v>
+        <v>630</v>
       </c>
       <c r="AL36" s="13" t="s">
-        <v>636</v>
+        <v>631</v>
       </c>
       <c r="AM36" s="13" t="s">
         <v>72</v>
@@ -7046,24 +7537,27 @@
         <v>74</v>
       </c>
       <c r="AQ36" s="13" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="37" spans="2:43" ht="409.6">
+      <c r="B37" s="13" t="s">
+        <v>576</v>
+      </c>
+      <c r="C37" s="17" t="s">
         <v>594</v>
       </c>
-    </row>
-    <row r="37" spans="2:43" ht="201.6">
-      <c r="B37" s="13" t="s">
-        <v>581</v>
-      </c>
-      <c r="C37" s="17" t="s">
-        <v>599</v>
-      </c>
       <c r="D37" s="14" t="s">
-        <v>603</v>
+        <v>598</v>
       </c>
       <c r="E37" s="17" t="s">
-        <v>607</v>
+        <v>602</v>
       </c>
       <c r="F37" s="17" t="s">
-        <v>519</v>
+        <v>518</v>
+      </c>
+      <c r="G37" s="14" t="s">
+        <v>661</v>
       </c>
       <c r="H37" s="13">
         <v>270</v>
@@ -7072,7 +7566,7 @@
         <v>350</v>
       </c>
       <c r="J37" s="17" t="s">
-        <v>623</v>
+        <v>618</v>
       </c>
       <c r="K37" s="13">
         <v>11</v>
@@ -7081,16 +7575,16 @@
         <v>5.5</v>
       </c>
       <c r="M37" s="17" t="s">
-        <v>637</v>
+        <v>632</v>
       </c>
       <c r="N37" s="13" t="s">
         <v>49</v>
       </c>
       <c r="O37" s="17" t="s">
-        <v>616</v>
+        <v>611</v>
       </c>
       <c r="P37" s="17" t="s">
-        <v>620</v>
+        <v>615</v>
       </c>
       <c r="S37" s="13" t="s">
         <v>85</v>
@@ -7108,7 +7602,7 @@
         <v>10</v>
       </c>
       <c r="X37" s="19" t="s">
-        <v>626</v>
+        <v>621</v>
       </c>
       <c r="Y37" s="16" t="s">
         <v>159</v>
@@ -7123,7 +7617,7 @@
         <v>61</v>
       </c>
       <c r="AC37" s="17" t="s">
-        <v>627</v>
+        <v>622</v>
       </c>
       <c r="AD37" s="13" t="s">
         <v>177</v>
@@ -7138,19 +7632,19 @@
         <v>66</v>
       </c>
       <c r="AH37" s="15" t="s">
-        <v>611</v>
+        <v>606</v>
       </c>
       <c r="AI37" s="13" t="s">
-        <v>638</v>
+        <v>633</v>
       </c>
       <c r="AJ37" s="13" t="s">
-        <v>637</v>
+        <v>632</v>
       </c>
       <c r="AK37" s="13" t="s">
-        <v>639</v>
+        <v>634</v>
       </c>
       <c r="AL37" s="17" t="s">
-        <v>640</v>
+        <v>635</v>
       </c>
       <c r="AM37" s="13" t="s">
         <v>72</v>
@@ -7165,7 +7659,7 @@
         <v>74</v>
       </c>
       <c r="AQ37" s="13" t="s">
-        <v>595</v>
+        <v>590</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: Adjust Morskie Oko visit duration for better plan composition
Changed time_min from 270 to 180 minutes and time_max from 350 to 270 minutes.
This allows the planning engine to include Morskie Oko in single-day plans
with 9-hour daily windows, as the previous duration (4.5-5.8h) was too long
to fit with other attractions.

Client approval received to match Dolina Kościeliska duration (180-270 min).
Expected scoring: Morskie Oko (95+35=130) > Dolina Kościeliska (88+35=123).
</commit_message>
<xml_diff>
--- a/data/zakopane.xlsx
+++ b/data/zakopane.xlsx
@@ -845,7 +845,7 @@
 </t>
         </is>
       </c>
-      <c r="AP2" t="b">
+      <c r="AP2" t="n">
         <v>0</v>
       </c>
       <c r="AQ2" t="inlineStr">
@@ -1054,7 +1054,7 @@
 </t>
         </is>
       </c>
-      <c r="AP3" t="b">
+      <c r="AP3" t="n">
         <v>0</v>
       </c>
       <c r="AQ3" t="inlineStr">
@@ -1263,7 +1263,7 @@
           <t>optional</t>
         </is>
       </c>
-      <c r="AP4" t="b">
+      <c r="AP4" t="n">
         <v>0</v>
       </c>
       <c r="AQ4" t="inlineStr">
@@ -1472,7 +1472,7 @@
 secondary</t>
         </is>
       </c>
-      <c r="AP5" t="b">
+      <c r="AP5" t="n">
         <v>0</v>
       </c>
       <c r="AQ5" t="inlineStr">
@@ -1680,7 +1680,7 @@
           <t>optional</t>
         </is>
       </c>
-      <c r="AP6" t="b">
+      <c r="AP6" t="n">
         <v>0</v>
       </c>
       <c r="AQ6" t="inlineStr">
@@ -1889,7 +1889,7 @@
           <t>optional</t>
         </is>
       </c>
-      <c r="AP7" t="b">
+      <c r="AP7" t="n">
         <v>0</v>
       </c>
       <c r="AQ7" t="inlineStr">
@@ -2099,7 +2099,7 @@
           <t>optional</t>
         </is>
       </c>
-      <c r="AP8" t="b">
+      <c r="AP8" t="n">
         <v>0</v>
       </c>
       <c r="AQ8" t="inlineStr">
@@ -2311,7 +2311,7 @@
           <t>optional</t>
         </is>
       </c>
-      <c r="AP9" t="b">
+      <c r="AP9" t="n">
         <v>0</v>
       </c>
       <c r="AQ9" t="inlineStr">
@@ -2519,7 +2519,7 @@
           <t>optional</t>
         </is>
       </c>
-      <c r="AP10" t="b">
+      <c r="AP10" t="n">
         <v>0</v>
       </c>
       <c r="AQ10" t="inlineStr">
@@ -2726,7 +2726,7 @@
           <t>optional</t>
         </is>
       </c>
-      <c r="AP11" t="b">
+      <c r="AP11" t="n">
         <v>0</v>
       </c>
       <c r="AQ11" t="inlineStr">
@@ -2930,7 +2930,7 @@
           <t>optional</t>
         </is>
       </c>
-      <c r="AP12" t="b">
+      <c r="AP12" t="n">
         <v>0</v>
       </c>
       <c r="AQ12" t="inlineStr">
@@ -3137,7 +3137,7 @@
           <t>optional</t>
         </is>
       </c>
-      <c r="AP13" t="b">
+      <c r="AP13" t="n">
         <v>0</v>
       </c>
       <c r="AQ13" t="inlineStr">
@@ -3389,7 +3389,7 @@
           <t>optional</t>
         </is>
       </c>
-      <c r="AP15" t="b">
+      <c r="AP15" t="n">
         <v>0</v>
       </c>
       <c r="AQ15" t="inlineStr">
@@ -3596,7 +3596,7 @@
           <t>optional</t>
         </is>
       </c>
-      <c r="AP16" t="b">
+      <c r="AP16" t="n">
         <v>1</v>
       </c>
       <c r="AQ16" t="inlineStr">
@@ -3804,7 +3804,7 @@
 secondary</t>
         </is>
       </c>
-      <c r="AP17" t="b">
+      <c r="AP17" t="n">
         <v>0</v>
       </c>
       <c r="AQ17" t="inlineStr">
@@ -4012,7 +4012,7 @@
 secondary</t>
         </is>
       </c>
-      <c r="AP18" t="b">
+      <c r="AP18" t="n">
         <v>0</v>
       </c>
       <c r="AQ18" t="inlineStr">
@@ -4220,7 +4220,7 @@
 secondary</t>
         </is>
       </c>
-      <c r="AP19" t="b">
+      <c r="AP19" t="n">
         <v>0</v>
       </c>
       <c r="AQ19" t="inlineStr">
@@ -4427,7 +4427,7 @@
           <t>secondary</t>
         </is>
       </c>
-      <c r="AP20" t="b">
+      <c r="AP20" t="n">
         <v>0</v>
       </c>
       <c r="AQ20" t="inlineStr">
@@ -4635,7 +4635,7 @@
 secondary</t>
         </is>
       </c>
-      <c r="AP21" t="b">
+      <c r="AP21" t="n">
         <v>0</v>
       </c>
       <c r="AQ21" t="inlineStr">
@@ -4842,7 +4842,7 @@
           <t>core</t>
         </is>
       </c>
-      <c r="AP22" t="b">
+      <c r="AP22" t="n">
         <v>0</v>
       </c>
       <c r="AQ22" t="inlineStr">
@@ -5050,7 +5050,7 @@
           <t>core</t>
         </is>
       </c>
-      <c r="AP23" t="b">
+      <c r="AP23" t="n">
         <v>0</v>
       </c>
       <c r="AQ23" t="inlineStr">
@@ -5257,7 +5257,7 @@
           <t>optional</t>
         </is>
       </c>
-      <c r="AP24" t="b">
+      <c r="AP24" t="n">
         <v>0</v>
       </c>
       <c r="AQ24" t="inlineStr">
@@ -5464,7 +5464,7 @@
           <t>optional</t>
         </is>
       </c>
-      <c r="AP25" t="b">
+      <c r="AP25" t="n">
         <v>0</v>
       </c>
       <c r="AQ25" t="inlineStr">
@@ -5670,7 +5670,7 @@
           <t>core</t>
         </is>
       </c>
-      <c r="AP26" t="b">
+      <c r="AP26" t="n">
         <v>0</v>
       </c>
       <c r="AQ26" t="inlineStr">
@@ -5876,7 +5876,7 @@
           <t>optional</t>
         </is>
       </c>
-      <c r="AP27" t="b">
+      <c r="AP27" t="n">
         <v>0</v>
       </c>
       <c r="AQ27" t="inlineStr">
@@ -6082,7 +6082,7 @@
           <t>secondary</t>
         </is>
       </c>
-      <c r="AP28" t="b">
+      <c r="AP28" t="n">
         <v>0</v>
       </c>
       <c r="AQ28" t="inlineStr">
@@ -6288,7 +6288,7 @@
           <t>secondary</t>
         </is>
       </c>
-      <c r="AP29" t="b">
+      <c r="AP29" t="n">
         <v>0</v>
       </c>
       <c r="AQ29" t="inlineStr">
@@ -6493,7 +6493,7 @@
           <t>secondary</t>
         </is>
       </c>
-      <c r="AP30" t="b">
+      <c r="AP30" t="n">
         <v>0</v>
       </c>
       <c r="AQ30" t="inlineStr">
@@ -6703,7 +6703,7 @@
           <t>optional</t>
         </is>
       </c>
-      <c r="AP31" t="b">
+      <c r="AP31" t="n">
         <v>0</v>
       </c>
       <c r="AQ31" t="inlineStr">
@@ -6910,7 +6910,7 @@
           <t>optional</t>
         </is>
       </c>
-      <c r="AP32" t="b">
+      <c r="AP32" t="n">
         <v>0</v>
       </c>
       <c r="AQ32" t="inlineStr">
@@ -7128,7 +7128,7 @@
           <t>secondary</t>
         </is>
       </c>
-      <c r="AP33" t="b">
+      <c r="AP33" t="n">
         <v>0</v>
       </c>
       <c r="AQ33" t="inlineStr">
@@ -7348,7 +7348,7 @@
           <t>core</t>
         </is>
       </c>
-      <c r="AP34" t="b">
+      <c r="AP34" t="n">
         <v>0</v>
       </c>
       <c r="AQ34" t="inlineStr">
@@ -7569,7 +7569,7 @@
           <t>core</t>
         </is>
       </c>
-      <c r="AP35" t="b">
+      <c r="AP35" t="n">
         <v>0</v>
       </c>
       <c r="AQ35" t="inlineStr">
@@ -7790,7 +7790,7 @@
           <t>core</t>
         </is>
       </c>
-      <c r="AP36" t="b">
+      <c r="AP36" t="n">
         <v>0</v>
       </c>
       <c r="AQ36" t="inlineStr">
@@ -7872,10 +7872,10 @@
         </is>
       </c>
       <c r="H37" t="n">
+        <v>180</v>
+      </c>
+      <c r="I37" t="n">
         <v>270</v>
-      </c>
-      <c r="I37" t="n">
-        <v>350</v>
       </c>
       <c r="J37" t="inlineStr">
         <is>
@@ -8011,7 +8011,7 @@
           <t>core</t>
         </is>
       </c>
-      <c r="AP37" t="b">
+      <c r="AP37" t="n">
         <v>0</v>
       </c>
       <c r="AQ37" t="inlineStr">

</xml_diff>

<commit_message>
feat: Add premium_experience flag and scoring penalty (CLIENT 08.02.2026)
- Add premium_experience column to zakopane.xlsx (KULIGI=TRUE)
- Implement calculate_premium_penalty() in budget.py:
  * Budget level 1 (budget): -40 penalty → almost excluded
  * Budget level 2 (standard): -20 penalty → occasionally suggested
  * Budget level 3+ (high): 0 penalty → normally suggested
- Integrate with engine.py scoring (after calculate_budget_score)
- Export from scoring/__init__.py (no duplication)
- Add premium_experience to load_zakopane.py loader
- Preserve premium_experience in normalizer.py
- Test: test_premium_experience.py - ALL 5 TESTS PASSED

CLIENT REQUIREMENT: KULIGI (247 PLN/osoba) should appear rarely at standard budget level, normally at high budget level.

No breaking changes. Backward compatible (non-premium POI unaffected).
</commit_message>
<xml_diff>
--- a/data/zakopane.xlsx
+++ b/data/zakopane.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -20,13 +20,16 @@
     <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
     <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -37,7 +40,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -45,12 +48,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -417,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AQ36"/>
+  <dimension ref="A1:AR36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -426,217 +438,222 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>ID</t>
         </is>
       </c>
-      <c r="B1" t="n">
+      <c r="B1" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Description_short</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Description_long</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Why visit</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Opening hours</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>opening_hours_seasonal</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>time_min</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>time_max</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Price</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>ticket_normal</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>ticket_reduced</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>Address</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Region</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Lat</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>Lng</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>Link do godzin</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>Link do cennika</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>Space</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>Intensity</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>weather_dependency</t>
         </is>
       </c>
-      <c r="V1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>popularity_score</t>
         </is>
       </c>
-      <c r="W1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>Must see score</t>
         </is>
       </c>
-      <c r="X1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>Peak hours</t>
         </is>
       </c>
-      <c r="Y1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>recommended_time_of_day</t>
         </is>
       </c>
-      <c r="Z1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>City</t>
         </is>
       </c>
-      <c r="AA1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>Target group</t>
         </is>
       </c>
-      <c r="AB1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>Children's age</t>
         </is>
       </c>
-      <c r="AC1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>Type of attraction</t>
         </is>
       </c>
-      <c r="AD1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>Activity_style</t>
         </is>
       </c>
-      <c r="AE1" t="inlineStr">
+      <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>crowd_level</t>
         </is>
       </c>
-      <c r="AF1" t="inlineStr">
+      <c r="AF1" s="1" t="inlineStr">
         <is>
           <t>Budget type</t>
         </is>
       </c>
-      <c r="AG1" t="inlineStr">
+      <c r="AG1" s="1" t="inlineStr">
         <is>
           <t>Seasonality of attractions</t>
         </is>
       </c>
-      <c r="AH1" t="inlineStr">
+      <c r="AH1" s="1" t="inlineStr">
         <is>
           <t>Pro_tip</t>
         </is>
       </c>
-      <c r="AI1" t="inlineStr">
+      <c r="AI1" s="1" t="inlineStr">
         <is>
           <t>parking_name</t>
         </is>
       </c>
-      <c r="AJ1" t="inlineStr">
+      <c r="AJ1" s="1" t="inlineStr">
         <is>
           <t>parking_address</t>
         </is>
       </c>
-      <c r="AK1" t="inlineStr">
+      <c r="AK1" s="1" t="inlineStr">
         <is>
           <t>parking_lat</t>
         </is>
       </c>
-      <c r="AL1" t="inlineStr">
+      <c r="AL1" s="1" t="inlineStr">
         <is>
           <t>parking_lng</t>
         </is>
       </c>
-      <c r="AM1" t="inlineStr">
+      <c r="AM1" s="1" t="inlineStr">
         <is>
           <t>parking_type</t>
         </is>
       </c>
-      <c r="AN1" t="inlineStr">
+      <c r="AN1" s="1" t="inlineStr">
         <is>
           <t>parking_walk_time_min</t>
         </is>
       </c>
-      <c r="AO1" t="inlineStr">
+      <c r="AO1" s="1" t="inlineStr">
         <is>
           <t>priority_level</t>
         </is>
       </c>
-      <c r="AP1" t="inlineStr">
+      <c r="AP1" s="1" t="inlineStr">
         <is>
           <t>kids_only</t>
         </is>
       </c>
-      <c r="AQ1" t="inlineStr">
+      <c r="AQ1" s="1" t="inlineStr">
         <is>
           <t>Tags</t>
+        </is>
+      </c>
+      <c r="AR1" s="1" t="inlineStr">
+        <is>
+          <t>premium_experience</t>
         </is>
       </c>
     </row>
@@ -853,6 +870,9 @@
           <t xml:space="preserve">mountain_culture, regional_heritage, workshop,themed_museum     </t>
         </is>
       </c>
+      <c r="AR2" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr"/>
@@ -1063,6 +1083,9 @@
 </t>
         </is>
       </c>
+      <c r="AR3" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr"/>
@@ -1271,6 +1294,9 @@
           <t xml:space="preserve">miniature_world, fairytale_world </t>
         </is>
       </c>
+      <c r="AR4" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr"/>
@@ -1480,6 +1506,9 @@
           <t>illusion_kids, interactive_exhibition_kids, interactive_exhibits,</t>
         </is>
       </c>
+      <c r="AR5" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr"/>
@@ -1689,6 +1718,9 @@
 </t>
         </is>
       </c>
+      <c r="AR6" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr"/>
@@ -1898,6 +1930,9 @@
 </t>
         </is>
       </c>
+      <c r="AR7" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr"/>
@@ -2036,7 +2071,7 @@
           <t>solo, couples, friends, family_kids</t>
         </is>
       </c>
-      <c r="AB8" s="1" t="n">
+      <c r="AB8" s="2" t="n">
         <v>41913</v>
       </c>
       <c r="AC8" t="inlineStr">
@@ -2106,6 +2141,9 @@
         <is>
           <t>snow_tubing, adrenaline_experience, beginner_friendly,group_activity</t>
         </is>
+      </c>
+      <c r="AR8" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -2319,6 +2357,9 @@
           <t>playground</t>
         </is>
       </c>
+      <c r="AR9" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr"/>
@@ -2527,6 +2568,9 @@
           <t>indoor_playroom, kids_obstacle_course, sensory_experience_kids</t>
         </is>
       </c>
+      <c r="AR10" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr"/>
@@ -2734,6 +2778,9 @@
           <t>indoor_playroom, kids_obstacle_course</t>
         </is>
       </c>
+      <c r="AR11" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr"/>
@@ -2938,6 +2985,9 @@
           <t>dinosaur_theme, walkthrough_experience, family_theme_park</t>
         </is>
       </c>
+      <c r="AR12" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr"/>
@@ -3145,6 +3195,9 @@
           <t>illusion_kids, interactive_exhibition_kids, science_center_kids</t>
         </is>
       </c>
+      <c r="AR13" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr"/>
@@ -3352,6 +3405,9 @@
           <t>illusion_kids, interactive_exhibition_kids</t>
         </is>
       </c>
+      <c r="AR14" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr"/>
@@ -3559,6 +3615,9 @@
           <t>playground, kids_obstacle_course</t>
         </is>
       </c>
+      <c r="AR15" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr"/>
@@ -3767,6 +3826,9 @@
           <t>thermal_baths, water_slides, family_friendly_water, spa_pools, sauna_zone</t>
         </is>
       </c>
+      <c r="AR16" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr"/>
@@ -3975,6 +4037,9 @@
           <t>thermal_baths, relax_zone, thermal_relax_focus, long_stay_possible, evening_relax</t>
         </is>
       </c>
+      <c r="AR17" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr"/>
@@ -4183,6 +4248,9 @@
           <t>thermal_baths, water_slides, kids_zone, sauna_zone, long_stay_possible</t>
         </is>
       </c>
+      <c r="AR18" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr"/>
@@ -4390,6 +4458,9 @@
           <t>thermal_baths, water_slides, kids_zone,  sauna_zone, spa_pools</t>
         </is>
       </c>
+      <c r="AR19" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr"/>
@@ -4598,6 +4669,9 @@
           <t>thermal_baths, water_slides, kids_zone, sauna_zone, long_stay_possible</t>
         </is>
       </c>
+      <c r="AR20" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr"/>
@@ -4805,6 +4879,9 @@
           <t>viewpoint, mountain_views, photo_spot, easy_access_nature</t>
         </is>
       </c>
+      <c r="AR21" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr"/>
@@ -5013,6 +5090,9 @@
           <t>themed_museum, multimedia_exhibition, interactive_exhibits</t>
         </is>
       </c>
+      <c r="AR22" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr"/>
@@ -5220,6 +5300,9 @@
           <t>themed_museum, interactive_exhibit, intimate_small_museum</t>
         </is>
       </c>
+      <c r="AR23" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr"/>
@@ -5427,6 +5510,9 @@
           <t>miniature_world, interactive_exhibition_kids, creative_workshops_kids</t>
         </is>
       </c>
+      <c r="AR24" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr"/>
@@ -5563,7 +5649,7 @@
           <t>solo, couples, friends, seniors</t>
         </is>
       </c>
-      <c r="AB25" s="1" t="n">
+      <c r="AB25" s="2" t="n">
         <v>41913</v>
       </c>
       <c r="AC25" t="inlineStr">
@@ -5632,6 +5718,9 @@
         <is>
           <t>regional_heritage, mountain_culture, temporary_exhibitions, multimedia_exhibition</t>
         </is>
+      </c>
+      <c r="AR25" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="26">
@@ -5769,7 +5858,7 @@
           <t>solo, couples, friends, family_kids, seniors</t>
         </is>
       </c>
-      <c r="AB26" s="1" t="n">
+      <c r="AB26" s="2" t="n">
         <v>41913</v>
       </c>
       <c r="AC26" t="inlineStr">
@@ -5838,6 +5927,9 @@
         <is>
           <t>composer_artist_house, historic_building, intimate_small_museum</t>
         </is>
+      </c>
+      <c r="AR26" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="27">
@@ -5975,7 +6067,7 @@
           <t>solo, couples, friends, family_kids, seniors</t>
         </is>
       </c>
-      <c r="AB27" s="1" t="n">
+      <c r="AB27" s="2" t="n">
         <v>41913</v>
       </c>
       <c r="AC27" t="inlineStr">
@@ -6044,6 +6136,9 @@
         <is>
           <t>architecture_heritage, mountain_culture, crafts_handicraft, historic_building</t>
         </is>
+      </c>
+      <c r="AR27" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="28">
@@ -6181,7 +6276,7 @@
           <t>solo, couples, friends, family_kids, seniors</t>
         </is>
       </c>
-      <c r="AB28" s="1" t="n">
+      <c r="AB28" s="2" t="n">
         <v>41913</v>
       </c>
       <c r="AC28" t="inlineStr">
@@ -6250,6 +6345,9 @@
         <is>
           <t>art_gallery, architecture_heritage, historic_building, temporary_exhibitions</t>
         </is>
+      </c>
+      <c r="AR28" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="29">
@@ -6386,7 +6484,7 @@
           <t>solo, couples, friends, family_kids, seniors</t>
         </is>
       </c>
-      <c r="AB29" s="1" t="n">
+      <c r="AB29" s="2" t="n">
         <v>41913</v>
       </c>
       <c r="AC29" t="inlineStr">
@@ -6455,6 +6553,9 @@
         <is>
           <t>composer_artist_house, historic_building, intimate_small_museum</t>
         </is>
+      </c>
+      <c r="AR29" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="30">
@@ -6666,6 +6767,9 @@
           <t>educational_farm, feeding_experience, educational_exhibition</t>
         </is>
       </c>
+      <c r="AR30" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr"/>
@@ -6872,6 +6976,9 @@
         <is>
           <t>architecture_heritage, mountain_culture, historic_building</t>
         </is>
+      </c>
+      <c r="AR31" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="32">
@@ -7090,6 +7197,9 @@
         <is>
           <t>horse_riding, low_intensity_activity, seasonal_activity, group_activity</t>
         </is>
+      </c>
+      <c r="AR32" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="33">
@@ -7310,6 +7420,9 @@
         <is>
           <t>must_see, nature_landscapes, hiking, scenic_views</t>
         </is>
+      </c>
+      <c r="AR33" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="34">
@@ -7532,6 +7645,9 @@
           <t>must_see, nature_landscapes, hiking, scenic_views</t>
         </is>
       </c>
+      <c r="AR34" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr"/>
@@ -7753,6 +7869,9 @@
           <t>easy_walk, family_friendly_trail, viewpoint_trail, out_and_back, trailhead_parking, stroller_friendly, crowd_prone</t>
         </is>
       </c>
+      <c r="AR35" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr"/>
@@ -7974,6 +8093,9 @@
           <t>must_see, nature_landscapes, hiking, easy_walk, long_distance, scenic_views</t>
         </is>
       </c>
+      <c r="AR36" t="b">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>